<commit_message>
add PV of dividends
</commit_message>
<xml_diff>
--- a/Homework/HW1/FIN514.xlsx
+++ b/Homework/HW1/FIN514.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanbaep2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanbaep2/Desktop/FIN514/Homework/HW1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
   <si>
     <t>Replicating Portfolio</t>
   </si>
@@ -238,9 +238,6 @@
     <t>Calculating Implied Volatility(Short Put)</t>
   </si>
   <si>
-    <t xml:space="preserve">*x1 and x2 stands for </t>
-  </si>
-  <si>
     <t>Spot</t>
   </si>
   <si>
@@ -293,6 +290,24 @@
   </si>
   <si>
     <t>Data which does not exist for exact maturity was calculated using linear interpolation.</t>
+  </si>
+  <si>
+    <t>Present Value</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Option Valuation(Using Black-Scholes Model)</t>
+  </si>
+  <si>
+    <t>Price of notes</t>
+  </si>
+  <si>
+    <t>Assumptions</t>
+  </si>
+  <si>
+    <t>*x1 and x2 stands for the point which is greatest lower bound (least upper bound) used for linear interpolation</t>
   </si>
 </sst>
 </file>
@@ -301,11 +316,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000%"/>
-    <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -377,13 +392,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,14 +408,31 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="blp_column_header" xfId="1"/>
@@ -1266,11 +1298,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1678716736"/>
-        <c:axId val="-1727563248"/>
+        <c:axId val="-1971451184"/>
+        <c:axId val="-1971448864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1678716736"/>
+        <c:axId val="-1971451184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1345,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1727563248"/>
+        <c:crossAx val="-1971448864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1322,7 +1354,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1727563248"/>
+        <c:axId val="-1971448864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1342,6 +1374,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1372,7 +1405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1678716736"/>
+        <c:crossAx val="-1971451184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2275,220 +2308,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I31"/>
+  <dimension ref="B2:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" t="s">
-        <v>86</v>
+      <c r="C2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="11">
+      <c r="B3" s="16">
         <v>43070</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="16">
         <v>43864</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="17">
         <f>(C3- B3) / 360</f>
         <v>2.2055555555555557</v>
       </c>
-      <c r="I3" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6">
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="18">
         <v>2635.03</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="17">
         <f>-LN('Caculation of Parameters'!C10) / 'Main Result'!D3</f>
         <v>1.9382664115765454E-2</v>
       </c>
+      <c r="D7" s="17">
+        <f>SUM(Dividend!E2:E27)</f>
+        <v>112.03308889355326</v>
+      </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>73</v>
-      </c>
+      <c r="B9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10">
-        <f>$B$6</f>
-        <v>2635.03</v>
+        <v>72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11">
-        <f>'Caculation of Parameters'!C17</f>
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="C11" s="14">
+        <f>$B$7</f>
+        <v>2635.03</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="14">
+        <f>1.1375 * $B$7</f>
+        <v>2997.3466250000001</v>
+      </c>
+      <c r="H11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="14">
+        <f>0.875 * $B$7</f>
+        <v>2305.6512500000003</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" t="e">
-        <f>(LN($B$6/C10)+($C$6+0.5*C11^2)*$D$3)/(C11*SQRT($D$3))</f>
-        <v>#DIV/0!</v>
+        <v>62</v>
+      </c>
+      <c r="C12" s="14">
+        <f>'Caculation of Parameters'!C17</f>
+        <v>0.1621856666666667</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="14">
+        <f>'Caculation of Parameters'!C23</f>
+        <v>0.13149627777777778</v>
+      </c>
+      <c r="H12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="14">
+        <f>'Caculation of Parameters'!C29</f>
+        <v>0.17952838888888889</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" t="e">
-        <f>C12 - C11 * SQRT($D$3)</f>
-        <v>#DIV/0!</v>
+        <v>77</v>
+      </c>
+      <c r="C13" s="14">
+        <f>(LN($B$7/C11)+($C$7+0.5*C12^2)*$D$3)/(C12*SQRT($D$3))</f>
+        <v>0.29791620649282535</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="14">
+        <f>(LN($B$7/F11)+($C$7+0.5*F12^2)*$D$3)/(F12*SQRT($D$3))</f>
+        <v>-0.34316178042659928</v>
+      </c>
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="14">
+        <f>(LN($B$7/I11)+($C$7+0.5*I12^2)*$D$3)/(I12*SQRT($D$3))</f>
+        <v>0.79447992824185787</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" t="e">
-        <f>$B$6 * _xlfn.NORM.DIST(C12, 0, 1, 1) - C10 * EXP(-$C$6 * $D$3) * _xlfn.NORM.DIST(C13, 0, 1, 1) - $D$6</f>
-        <v>#DIV/0!</v>
+        <v>78</v>
+      </c>
+      <c r="C14" s="14">
+        <f>C13 - C12 * SQRT($D$3)</f>
+        <v>5.7052441201828952E-2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="14">
+        <f>F13 - F12 * SQRT($D$3)</f>
+        <v>-0.53844838767286018</v>
+      </c>
+      <c r="H14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="14">
+        <f>I13 - I12 * SQRT($D$3)</f>
+        <v>0.52786029030999759</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="14">
+        <f>$B$7 * _xlfn.NORM.DIST(C13, 0, 1, 1) - C11 * EXP(-$C$7 * $D$3) * _xlfn.NORM.DIST(C14, 0, 1, 1) - $D$7</f>
+        <v>194.27457379104379</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="14">
+        <f>$B$7 * _xlfn.NORM.DIST(F13, 0, 1, 1) - F11 * EXP(-$C$7 * $D$3) * _xlfn.NORM.DIST(F14, 0, 1, 1) - $D$7</f>
+        <v>4.1004064234601429</v>
+      </c>
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="14">
+        <f>-$B$7 * _xlfn.NORM.DIST(-I13, 0, 1, 1) + I11 * EXP(-$C$7 * $D$3) * _xlfn.NORM.DIST(-I14, 0, 1, 1) + D7</f>
+        <v>209.65851137279736</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17">
-        <f>1.1375 * B6</f>
-        <v>2997.3466250000001</v>
+        <v>87</v>
+      </c>
+      <c r="C16">
+        <v>1.6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16">
+        <v>-1.6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>87</v>
+      </c>
+      <c r="I16">
+        <v>-1.1429</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18">
-        <f>'Caculation of Parameters'!C23</f>
-        <v>9.5698777777777758E-2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19">
-        <f>(LN($B$6/C17)+($C$6+0.5*C18^2)*$D$3)/(C18*SQRT($D$3))</f>
-        <v>-0.53463287835085349</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20">
-        <f>C19 - C18 * SQRT($D$3)</f>
-        <v>-0.67675621405027953</v>
+        <v>74</v>
+      </c>
+      <c r="C19" s="19">
+        <f>1000 * 'Caculation of Parameters'!C10</f>
+        <v>958.15133618483571</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21">
-        <f>$B$6 * _xlfn.NORM.DIST(C19, 0, 1, 1) - C17 * EXP(-$C$6 * $D$3) * _xlfn.NORM.DIST(C20, 0, 1, 1) - $D$6</f>
-        <v>65.248510073851548</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24">
-        <f>0.875 * B6</f>
-        <v>2305.6512500000003</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25">
-        <f>'Caculation of Parameters'!C29</f>
-        <v>0.14373088888888885</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="19">
+        <f>C16*C15 + F16*F15 + I16*I15 + C19</f>
+        <v>1022.8112913249995</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26">
-        <f>(LN($B$6/C24)+($C$6+0.5*C25^2)*$D$3)/(C25*SQRT($D$3))</f>
-        <v>0.93256879001960902</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27">
-        <f>C26 - C25 * SQRT($D$3)</f>
-        <v>0.71911242363458361</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28">
-        <f>-$B$6 * _xlfn.NORM.DIST(-C26, 0, 1, 1) + C24 * EXP(-$C$6 * $D$3) * _xlfn.NORM.DIST(-C27, 0, 1, 1) + D6</f>
-        <v>58.937611575654216</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
@@ -2496,16 +2590,11 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31">
-        <f>1000 * 'Caculation of Parameters'!C10</f>
-        <v>958.15133618483571</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2513,10 +2602,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="B2:F37"/>
+  <dimension ref="B2:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2572,13 +2661,13 @@
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
@@ -2661,13 +2750,13 @@
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
@@ -2698,11 +2787,11 @@
       </c>
       <c r="E15" s="10">
         <f>INDEX('Implied Volatility'!$C$4:$H$4,0,MATCH('Caculation of Parameters'!$C$3-'Caculation of Parameters'!$B$3, 'Implied Volatility'!$C$2:$H$2,1) - 1)</f>
-        <v>0</v>
+        <v>0.15909000000000001</v>
       </c>
       <c r="F15" s="10">
         <f>($D$16 - $D$3) / ($D$16 - $D$15) * E15</f>
-        <v>0</v>
+        <v>0.12638816666666666</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
@@ -2716,11 +2805,11 @@
       </c>
       <c r="E16" s="10">
         <f>INDEX('Implied Volatility'!$C$4:$H$4,0,MATCH('Caculation of Parameters'!$C$3-'Caculation of Parameters'!$B$3, 'Implied Volatility'!$C$2:$H$2,1) )</f>
-        <v>0</v>
+        <v>0.17415</v>
       </c>
       <c r="F16" s="10">
         <f>($D$3-$D$15) / ($D$16 - $D$15) * $E$16</f>
-        <v>0</v>
+        <v>3.5797500000000031E-2</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -2729,7 +2818,7 @@
       </c>
       <c r="C17" s="10">
         <f>SUM(F15:F16)</f>
-        <v>0</v>
+        <v>0.1621856666666667</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -2743,13 +2832,13 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
@@ -2802,7 +2891,7 @@
       </c>
       <c r="F22" s="10">
         <f>($D$3-$D$15) / ($D$16 - $D$15) * $E$16</f>
-        <v>0</v>
+        <v>3.5797500000000031E-2</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
@@ -2811,7 +2900,7 @@
       </c>
       <c r="C23" s="10">
         <f>SUM(F21:F22)</f>
-        <v>9.5698777777777758E-2</v>
+        <v>0.13149627777777778</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -2825,13 +2914,13 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
@@ -2884,7 +2973,7 @@
       </c>
       <c r="F28" s="10">
         <f>($D$3-$D$15) / ($D$16 - $D$15) * $E$16</f>
-        <v>0</v>
+        <v>3.5797500000000031E-2</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
@@ -2893,7 +2982,7 @@
       </c>
       <c r="C29" s="10">
         <f>SUM(F27:F28)</f>
-        <v>0.14373088888888885</v>
+        <v>0.17952838888888889</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -2907,15 +2996,13 @@
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="15" t="s">
+        <v>91</v>
+      </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="6" t="s">
-        <v>68</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6139,19 +6226,19 @@
         <v>100</v>
       </c>
       <c r="D124">
-        <f t="shared" ref="D124:D134" si="20">1.6 *MAX(0, B124-$B$9)</f>
+        <f t="shared" ref="D124:D132" si="20">1.6 *MAX(0, B124-$B$9)</f>
         <v>64</v>
       </c>
       <c r="E124">
-        <f t="shared" ref="E124:E134" si="21">-1.6*MAX(0, B124 - 1.1375 *$B$9)</f>
+        <f t="shared" ref="E124:E132" si="21">-1.6*MAX(0, B124 - 1.1375 *$B$9)</f>
         <v>-42</v>
       </c>
       <c r="F124">
-        <f t="shared" ref="F124:F134" si="22">-1.1429 *MAX(0, 0.875*$B$9 - B124)</f>
+        <f t="shared" ref="F124:F132" si="22">-1.1429 *MAX(0, 0.875*$B$9 - B124)</f>
         <v>0</v>
       </c>
       <c r="G124">
-        <f t="shared" ref="G124:G134" si="23">SUM(C124:F124)</f>
+        <f t="shared" ref="G124:G132" si="23">SUM(C124:F124)</f>
         <v>122</v>
       </c>
     </row>
@@ -6160,7 +6247,7 @@
         <v>1.4125000000000001</v>
       </c>
       <c r="B125">
-        <f t="shared" ref="B125:B134" si="24">A125*$B$9</f>
+        <f t="shared" ref="B125:B132" si="24">A125*$B$9</f>
         <v>141.25</v>
       </c>
       <c r="C125">
@@ -6388,16 +6475,19 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -6407,301 +6497,508 @@
       <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>43100</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <f>AVERAGE(C14,C26)</f>
         <v>4.6135000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="13">
+        <f>EXP(LN('Term Structure'!$G$4) / (('Term Structure'!$A$4 - 'Term Structure'!$A$2) / 360) * ((A2 - 'Term Structure'!$A$2) / 360))</f>
+        <v>0.99881040663472931</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>4.608011811009324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>43131</v>
       </c>
       <c r="B3">
         <v>26</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>0.50600000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="13">
+        <f>EXP(LN('Term Structure'!$G$4) / (('Term Structure'!$A$4 - 'Term Structure'!$A$2) / 360) * ((A3 - 'Term Structure'!$A$2) / 360))</f>
+        <v>0.99758264681280484</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E27" si="0">C3*D3</f>
+        <v>0.50477681928727924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43159</v>
       </c>
       <c r="B4">
         <v>164</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>5.7629999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="13">
+        <f>EXP(LN('Term Structure'!$G$4) / (('Term Structure'!$A$4 - 'Term Structure'!$A$2) / 360) * ((A4 - 'Term Structure'!$A$2) / 360))</f>
+        <v>0.9964749996895429</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>5.742685423210836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>43190</v>
       </c>
       <c r="B5">
         <v>170</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>4.0049999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f>((A5-'Term Structure'!$A$5)/360)/(('Term Structure'!$A$6-'Term Structure'!$A$5)/360)*'Term Structure'!$G$6+(('Term Structure'!$A$6-Dividend!A5)/360)/ (('Term Structure'!$A$6-'Term Structure'!$A$5)/360) * 'Term Structure'!$G$5</f>
+        <v>0.99500267617874183</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>3.984985718095861</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>43220</v>
       </c>
       <c r="B6">
         <v>80</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>3.1739999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f>((A6-'Term Structure'!$A$5)/360)/(('Term Structure'!$A$6-'Term Structure'!$A$5)/360)*'Term Structure'!$G$6+(('Term Structure'!$A$6-Dividend!A6)/360)/ (('Term Structure'!$A$6-'Term Structure'!$A$5)/360) * 'Term Structure'!$G$5</f>
+        <v>0.9935784028512934</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3.1536178506500052</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>43251</v>
       </c>
       <c r="B7">
         <v>182</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>6.18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f>((A7-'Term Structure'!$A$5)/360)/(('Term Structure'!$A$6-'Term Structure'!$A$5)/360)*'Term Structure'!$G$6+(('Term Structure'!$A$6-Dividend!A7)/360)/ (('Term Structure'!$A$6-'Term Structure'!$A$5)/360) * 'Term Structure'!$G$5</f>
+        <v>0.99210665374626328</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>6.1312191201519068</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>43281</v>
       </c>
       <c r="B8">
         <v>157</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>3.9140000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f>((A8 - 'Term Structure'!$A$6) / 360) / (('Term Structure'!$A$7 - 'Term Structure'!$A$6) / 360) * 'Term Structure'!$G$7 + (('Term Structure'!$A$7 - Dividend!A8) / 360) / (('Term Structure'!$A$7 - 'Term Structure'!$A$6) / 360) * 'Term Structure'!$G$6</f>
+        <v>0.99064239498679763</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>3.877374333978326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>43312</v>
       </c>
       <c r="B9">
         <v>75</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>3.0510000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f>((A9 - 'Term Structure'!$A$6) / 360) / (('Term Structure'!$A$7 - 'Term Structure'!$A$6) / 360) * 'Term Structure'!$G$7 + (('Term Structure'!$A$7 - Dividend!A9) / 360) / (('Term Structure'!$A$7 - 'Term Structure'!$A$6) / 360) * 'Term Structure'!$G$6</f>
+        <v>0.98904669104251419</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3.0175814543707111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>43343</v>
       </c>
       <c r="B10">
         <v>182</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>6.0309999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f>((A10 - 'Term Structure'!$A$6) / 360) / (('Term Structure'!$A$7 - 'Term Structure'!$A$6) / 360) * 'Term Structure'!$G$7 + (('Term Structure'!$A$7 - Dividend!A10) / 360) / (('Term Structure'!$A$7 - 'Term Structure'!$A$6) / 360) * 'Term Structure'!$G$6</f>
+        <v>0.98745098709823054</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>5.955316903189428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>43373</v>
       </c>
       <c r="B11">
         <v>151</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>3.895</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f>((A11 - 'Term Structure'!$A$7) / 360) / (('Term Structure'!$A$8 - 'Term Structure'!$A$7) / 360) * 'Term Structure'!$G$8 + (('Term Structure'!$A$8 - Dividend!A11) / 360) / (('Term Structure'!$A$8 - 'Term Structure'!$A$7) / 360) * 'Term Structure'!$G$7</f>
+        <v>0.98588143571522613</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>3.8400081921108056</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>43404</v>
       </c>
       <c r="B12">
         <v>76</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>3.0790000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f>((A12 - 'Term Structure'!$A$7) / 360) / (('Term Structure'!$A$8 - 'Term Structure'!$A$7) / 360) * 'Term Structure'!$G$8 + (('Term Structure'!$A$8 - Dividend!A12) / 360) / (('Term Structure'!$A$8 - 'Term Structure'!$A$7) / 360) * 'Term Structure'!$G$7</f>
+        <v>0.98421437044870386</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>3.0303960466115591</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>43434</v>
       </c>
       <c r="B13">
         <v>186</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>6.4569999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f>((A13 - 'Term Structure'!$A$7) / 360) / (('Term Structure'!$A$8 - 'Term Structure'!$A$7) / 360) * 'Term Structure'!$G$8 + (('Term Structure'!$A$8 - Dividend!A13) / 360) / (('Term Structure'!$A$8 - 'Term Structure'!$A$7) / 360) * 'Term Structure'!$G$7</f>
+        <v>0.98260108148110159</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>6.3446551831234732</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>43465</v>
       </c>
       <c r="B14">
         <v>158</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>4.2160000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f>((Dividend!A14 - 'Term Structure'!$A$8) / 360) / (('Term Structure'!$A$9 - 'Term Structure'!$A$8) / 360) * 'Term Structure'!$G$9 + (('Term Structure'!$A$9 - Dividend!A14) / 360) / (('Term Structure'!$A$9 - 'Term Structure'!$A$8) / 360) * 'Term Structure'!$G$8</f>
+        <v>0.98091018061366553</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>4.1355173214672138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>43496</v>
       </c>
       <c r="B15">
         <v>79</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>3.5579999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f>((Dividend!A15 - 'Term Structure'!$A$8) / 360) / (('Term Structure'!$A$9 - 'Term Structure'!$A$8) / 360) * 'Term Structure'!$G$9 + (('Term Structure'!$A$9 - Dividend!A15) / 360) / (('Term Structure'!$A$9 - 'Term Structure'!$A$8) / 360) * 'Term Structure'!$G$8</f>
+        <v>0.97918154004478319</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>3.4839279194793384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>43524</v>
       </c>
       <c r="B16">
         <v>167</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <v>6.016</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f>((Dividend!A16 - 'Term Structure'!$A$8) / 360) / (('Term Structure'!$A$9 - 'Term Structure'!$A$8) / 360) * 'Term Structure'!$G$9 + (('Term Structure'!$A$9 - Dividend!A16) / 360) / (('Term Structure'!$A$9 - 'Term Structure'!$A$8) / 360) * 'Term Structure'!$G$8</f>
+        <v>0.97762018727288924</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>5.8813630466337017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>43555</v>
       </c>
       <c r="B17">
         <v>162</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>3.968</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <f>((A17 - 'Term Structure'!$A$9) / 360) / (('Term Structure'!$A$10 - 'Term Structure'!$A$9) / 360) * 'Term Structure'!$G$10 + (('Term Structure'!$A$10 - Dividend!A17) / 360) / (('Term Structure'!$A$10 - 'Term Structure'!$A$9) / 360) * 'Term Structure'!$G$9</f>
+        <v>0.97587901823591283</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>3.8722879443601022</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>43585</v>
       </c>
       <c r="B18">
         <v>78</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>3.2189999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <f>((A18 - 'Term Structure'!$A$9) / 360) / (('Term Structure'!$A$10 - 'Term Structure'!$A$9) / 360) * 'Term Structure'!$G$10 + (('Term Structure'!$A$10 - Dividend!A18) / 360) / (('Term Structure'!$A$10 - 'Term Structure'!$A$9) / 360) * 'Term Structure'!$G$9</f>
+        <v>0.97417197171667946</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>3.1358595769559909</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>43616</v>
       </c>
       <c r="B19">
         <v>182</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>6.4960000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f>((A19 - 'Term Structure'!$A$9) / 360) / (('Term Structure'!$A$10 - 'Term Structure'!$A$9) / 360) * 'Term Structure'!$G$10 + (('Term Structure'!$A$10 - Dividend!A19) / 360) / (('Term Structure'!$A$10 - 'Term Structure'!$A$9) / 360) * 'Term Structure'!$G$9</f>
+        <v>0.97240802364680512</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>6.3167625216096468</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>43646</v>
       </c>
       <c r="B20">
         <v>155</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="11">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <f>((A20 - 'Term Structure'!$A$10) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$11 + (('Term Structure'!$A$11 - Dividend!A20) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$10</f>
+        <v>0.97069908323224074</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>4.2710759662218596</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>43677</v>
       </c>
       <c r="B21">
         <v>80</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <v>3.2160000000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <f>((A21 - 'Term Structure'!$A$10) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$11 + (('Term Structure'!$A$11 - Dividend!A21) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$10</f>
+        <v>0.96892979782097877</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>3.1160782297922678</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>43708</v>
       </c>
       <c r="B22">
         <v>176</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <v>6.4189999999999996</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <f>((A22 - 'Term Structure'!$A$10) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$11 + (('Term Structure'!$A$11 - Dividend!A22) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$10</f>
+        <v>0.9671605124097169</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>6.2082033291579721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>43738</v>
       </c>
       <c r="B23">
         <v>157</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <v>4.3239999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <f>((A23 - 'Term Structure'!$A$10) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$11 + (('Term Structure'!$A$11 - Dividend!A23) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$10</f>
+        <v>0.96544830072139876</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>4.1745984523193282</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>43769</v>
       </c>
       <c r="B24">
         <v>76</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="11">
         <v>3.2559999999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <f>((A24 - 'Term Structure'!$A$10) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$11 + (('Term Structure'!$A$11 - Dividend!A24) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$10</f>
+        <v>0.96367901531013678</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>3.1377388738498051</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>43799</v>
       </c>
       <c r="B25">
         <v>181</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="11">
         <v>6.5919999999999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <f>((A25 - 'Term Structure'!$A$10) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$11 + (('Term Structure'!$A$11 - Dividend!A25) / 360) / (('Term Structure'!$A$11 - 'Term Structure'!$A$10) / 360) * 'Term Structure'!$G$10</f>
+        <v>0.96196680362181863</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>6.3412851694750278</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>43830</v>
       </c>
       <c r="B26">
         <v>160</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <v>5.0110000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <f xml:space="preserve"> ((A26 - 'Term Structure'!$A$11) / 360) / (('Term Structure'!$A$12 - 'Term Structure'!$A$11) / 360) * 'Term Structure'!$G$12 + (('Term Structure'!$A$12 - Dividend!A26) / 360) / (('Term Structure'!$A$12 - 'Term Structure'!$A$11) / 360) * 'Term Structure'!$G$11</f>
+        <v>0.96015172551745165</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>4.81132029656795</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>43861</v>
       </c>
       <c r="B27">
         <v>76</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="11">
         <v>3.085</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>43890</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" s="12">
-        <v>7.9000000000000001E-2</v>
-      </c>
+      <c r="D27">
+        <f xml:space="preserve"> ((A27 - 'Term Structure'!$A$11) / 360) / (('Term Structure'!$A$12 - 'Term Structure'!$A$11) / 360) * 'Term Structure'!$G$12 + (('Term Structure'!$A$12 - Dividend!A27) / 360) / (('Term Structure'!$A$12 - 'Term Structure'!$A$11) / 360) * 'Term Structure'!$G$11</f>
+        <v>0.95832784112594904</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>2.9564413898735529</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="C28" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6711,26 +7008,29 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <f>'Caculation of Parameters'!B3</f>
         <v>43070</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -6756,7 +7056,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -6782,8 +7082,9 @@
       <c r="H4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
@@ -6810,7 +7111,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -6837,7 +7138,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -6864,7 +7165,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
@@ -6891,7 +7192,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -6918,7 +7219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -6945,7 +7246,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
@@ -6972,7 +7273,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>31</v>
       </c>
@@ -6999,7 +7300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>32</v>
       </c>
@@ -7026,7 +7327,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
@@ -7053,7 +7354,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
@@ -7080,7 +7381,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
@@ -7414,9 +7715,7 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -7532,21 +7831,45 @@
       <c r="B4">
         <v>100</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="C4" s="2">
+        <v>8.9849999999999999E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.1211</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.13996</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.15065000000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.15909000000000001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.17415</v>
+      </c>
       <c r="J4">
         <v>100</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="K4" s="2">
+        <v>8.6099999999999996E-2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.11703</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.13539999999999999</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.14316000000000001</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.14956</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.16511000000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5">
@@ -7650,12 +7973,24 @@
       <c r="B10">
         <v>100</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="C10" s="2">
+        <v>8.6099999999999996E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.11703</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.13539999999999999</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.14316000000000001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.14956</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.16511000000000001</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11">

</xml_diff>